<commit_message>
new data added to excel
</commit_message>
<xml_diff>
--- a/data_motherconferences/review_ecological conferences.XLSX
+++ b/data_motherconferences/review_ecological conferences.XLSX
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="childcare" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>Group of measures</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>&gt;500</t>
-  </si>
-  <si>
-    <t>number of keynotes</t>
   </si>
   <si>
     <t>USA</t>
@@ -201,13 +198,25 @@
   </si>
   <si>
     <t>Is there a reduction fees for families attending the conference?</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Childcare is provided by a licensed, bonded, and insured childcare company, Kiddie Corp. ESA has been partnering with Kiddie Corp for many years to provide an on-site childcare program for our attendees. The program is open for children ages six months to 12 years.</t>
+  </si>
+  <si>
+    <t>number of keynote speakers</t>
+  </si>
+  <si>
+    <t>female keynote speakers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +231,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Georgia"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,12 +268,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,16 +572,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,64 +595,64 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -625,215 +662,231 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="11.5546875" style="4"/>
+    <col min="8" max="8" width="35.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="11.5546875" style="4"/>
+    <col min="17" max="17" width="32.5546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5">
+        <v>45109</v>
+      </c>
+      <c r="F2" s="5">
+        <v>45113</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45144</v>
+      </c>
+      <c r="F3" s="5">
+        <v>45149</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="M3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5">
+        <v>45130</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45134</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45109</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45113</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="5">
+        <v>45272</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45275</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45144</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45149</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45130</v>
-      </c>
-      <c r="F4" s="1">
-        <v>45134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4">
-        <v>4</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H6" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45272</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45275</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <v>1200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data added to excel table
</commit_message>
<xml_diff>
--- a/data_motherconferences/review_ecological conferences.XLSX
+++ b/data_motherconferences/review_ecological conferences.XLSX
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B534319-34D1-4906-AB09-9837BDE0B307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="childcare" sheetId="1" r:id="rId1"/>
     <sheet name="conferences" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>Group of measures</t>
   </si>
@@ -91,9 +92,6 @@
     <t>expected number of attendants</t>
   </si>
   <si>
-    <t>&gt;500</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
@@ -104,9 +102,6 @@
   </si>
   <si>
     <t>https://ecologicalsocietyofamerica.org/portland2023/</t>
-  </si>
-  <si>
-    <t>website code of conduct</t>
   </si>
   <si>
     <t>https://ecologicalsocietyofamerica.org/events/code-of-conduct-for-esa-events/</t>
@@ -210,12 +205,51 @@
   </si>
   <si>
     <t>female keynote speakers</t>
+  </si>
+  <si>
+    <t>&gt;400</t>
+  </si>
+  <si>
+    <t>atbc2023@tropicalbio.org</t>
+  </si>
+  <si>
+    <t>Wrote them asking for children facilities</t>
+  </si>
+  <si>
+    <t>ECONET2023</t>
+  </si>
+  <si>
+    <t>PHENOLOGY2022</t>
+  </si>
+  <si>
+    <t>ATBC2022</t>
+  </si>
+  <si>
+    <t>website_codeconduct</t>
+  </si>
+  <si>
+    <t>https://www.atbc2023.org/codeofconduct</t>
+  </si>
+  <si>
+    <t>https://www.atbc2022.org/</t>
+  </si>
+  <si>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Conserving Tropical Biodiversity and Achieving Socio-Ecological Resilience in the Anthropocene:​ Opportunities and Challenges</t>
+  </si>
+  <si>
+    <t>https://www.atbc2022.org/codeofconduct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,19 +603,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,64 +629,64 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -661,25 +695,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.5546875" style="4"/>
-    <col min="8" max="8" width="35.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="11.5546875" style="4"/>
-    <col min="17" max="17" width="32.5546875" style="4" customWidth="1"/>
+    <col min="1" max="7" width="11.5703125" style="4"/>
+    <col min="8" max="8" width="35.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.5703125" style="4"/>
+    <col min="12" max="12" width="23.85546875" style="4" customWidth="1"/>
+    <col min="13" max="15" width="11.5703125" style="4"/>
+    <col min="16" max="16" width="22.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="35.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -714,25 +751,25 @@
         <v>16</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -755,7 +792,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>15</v>
@@ -766,25 +803,37 @@
       <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="N2" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="O2" s="4">
+        <v>4</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="5">
         <v>45144</v>
@@ -796,39 +845,39 @@
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="E4" s="5">
         <v>45130</v>
@@ -837,42 +886,42 @@
         <v>45134</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N4" s="4">
         <v>4</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E6" s="5">
         <v>45272</v>
@@ -884,15 +933,63 @@
         <v>12</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M6" s="4">
         <v>1200</v>
       </c>
     </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="5">
+        <v>44752</v>
+      </c>
+      <c r="F9" s="5">
+        <v>44756</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1" display="mailto:jaciglia@cedarcrest.edu"/>
+    <hyperlink ref="P4" r:id="rId1" display="mailto:jaciglia@cedarcrest.edu" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
more conferences added to database
</commit_message>
<xml_diff>
--- a/data_motherconferences/review_ecological conferences.XLSX
+++ b/data_motherconferences/review_ecological conferences.XLSX
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F3BCB-A30B-4332-B994-F9FF81841331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AD0EBB-101A-4230-B987-9DB94DBF83EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="childcare" sheetId="1" r:id="rId1"/>
-    <sheet name="conferences" sheetId="2" r:id="rId2"/>
-    <sheet name="metadata" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId2"/>
+    <sheet name="conferences" sheetId="2" r:id="rId3"/>
+    <sheet name="metadata" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="101">
   <si>
     <t>Group of measures</t>
   </si>
@@ -262,9 +263,6 @@
     <t>Is there a discount for parent registration?</t>
   </si>
   <si>
-    <t>GFO</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -296,13 +294,46 @@
   </si>
   <si>
     <t>485 $</t>
+  </si>
+  <si>
+    <t>Not said</t>
+  </si>
+  <si>
+    <t>Yes, half price</t>
+  </si>
+  <si>
+    <t>GFO2023</t>
+  </si>
+  <si>
+    <t>The Future of Biodiversity – overcoming barriers of taxa, realms and scales</t>
+  </si>
+  <si>
+    <t>https://www.gfoe-conference.de/</t>
+  </si>
+  <si>
+    <t>Leipizig</t>
+  </si>
+  <si>
+    <t>Does the conference have a code of conduct?</t>
+  </si>
+  <si>
+    <t>not said</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +369,20 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -360,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,6 +439,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -675,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,7 +734,7 @@
     <col min="2" max="2" width="46.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,27 +750,39 @@
       <c r="E1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -731,80 +790,166 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>450</v>
+      </c>
+      <c r="E10">
+        <v>480</v>
+      </c>
+      <c r="F10">
+        <v>450</v>
+      </c>
+      <c r="G10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>77</v>
       </c>
     </row>
@@ -815,14 +960,213 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DBFD69-E82C-47CC-AF73-96198F569FC2}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,7 +1188,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
@@ -862,7 +1206,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>10</v>
@@ -871,7 +1215,7 @@
         <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>13</v>
@@ -889,7 +1233,7 @@
         <v>21</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>58</v>
@@ -898,10 +1242,10 @@
         <v>59</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>35</v>
@@ -942,7 +1286,7 @@
         <v>46</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>14</v>
@@ -1001,7 +1345,7 @@
         <v>47</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>27</v>
@@ -1019,7 +1363,7 @@
         <v>28</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T3" s="4" t="s">
         <v>11</v>
@@ -1110,6 +1454,9 @@
       <c r="I6" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
@@ -1186,7 +1533,22 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>4</v>
+      </c>
+      <c r="R10" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B876F3-34C3-4A9D-AEA2-CEEA558224A7}">
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -1213,18 +1575,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1254,7 +1616,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1269,7 +1631,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1299,7 +1661,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
@@ -1314,12 +1676,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>